<commit_message>
Agremamos librerias necesarias , // comenzar con el envio a whatsapp
</commit_message>
<xml_diff>
--- a/emails.xlsx
+++ b/emails.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,6 +484,91 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba en Excel </t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba en Excel 1 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba en Excel </t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba en Excel 1 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba en Excel </t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba en Excel 1 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba en Excel </t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba en Excel 1 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba en Excel </t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba en Excel 1 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Mejora en ejecucion del envio a whatsapp/twilio
</commit_message>
<xml_diff>
--- a/emails.xlsx
+++ b/emails.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -961,6 +961,380 @@
         </is>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automatizacion Gmail/whatasapp </t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba automatizacion Gmail/whatasapp </t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automatizacion Gmail/whatasapp </t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba automatizacion Gmail/whatasapp </t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automatizacion Gmail/whatasapp </t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba automatizacion Gmail/whatasapp </t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automatizacion Gmail/whatasapp </t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba automatizacion Gmail/whatasapp </t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automatizacion Gmail/whatasapp </t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba automatizacion Gmail/whatasapp </t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automatizacion Gmail/whatasapp </t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba automatizacion Gmail/whatasapp </t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automatizacion Gmail/whatasapp </t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba automatizacion Gmail/whatasapp </t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automatizacion Gmail/whatasapp </t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba automatizacion Gmail/whatasapp </t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automatizacion Gmail/whatasapp </t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba automatizacion Gmail/whatasapp </t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automatizacion Gmail/whatasapp </t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba automatizacion Gmail/whatasapp </t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automatizacion Gmail/whatasapp </t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba automatizacion Gmail/whatasapp </t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automatizacion Gmail/whatasapp </t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba automatizacion Gmail/whatasapp </t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automatizacion Gmail/whatasapp </t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba automatizacion Gmail/whatasapp </t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automatizacion Gmail/whatasapp </t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba automatizacion Gmail/whatasapp </t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automatizacion Gmail/whatasapp </t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba automatizacion Gmail/whatasapp </t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba con renata</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba con renata </t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba con renata</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba con renata </t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Archivos creados por ejecucion en env
</commit_message>
<xml_diff>
--- a/emails.xlsx
+++ b/emails.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1335,6 +1335,28 @@
         </is>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba con renata</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba con renata </t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Se organizo en funciones / avance de que se envia cada 1min automaticamente
</commit_message>
<xml_diff>
--- a/emails.xlsx
+++ b/emails.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D191"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1357,6 +1357,3284 @@
         </is>
       </c>
     </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba con renata</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba con renata </t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automa</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba automa Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automa</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba automa Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automa 2</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba 2 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automa 2</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba 2 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automa 2</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba 2 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automa 2</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba 2 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automa 2</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba 2 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automa 2</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba 2 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automa 2</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba 2 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automa 2</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba 2 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automa 2</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba 2 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automa 2</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba 2 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automa 2</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba 2 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automa 2</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba 2 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automa 2</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba 2 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automa 2</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba 2 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automa 2</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba 2 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automa 2</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba 2 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automa 2</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba 2 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automa 2</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba 2 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automa 2</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba 2 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automa 2</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba 2 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automa 2</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba 2 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automa 2</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba 2 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automa 2</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba 2 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automa 2</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba 2 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automa 2</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba 2 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automa 2</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba 2 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automa 2</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba 2 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automa 2</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba 2 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automa 2</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba 2 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automa 2</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba 2 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automa 2</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba 2 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automa 2</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba 2 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automa 2</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba 2 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automa 2</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba 2 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automa 2</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba 2 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automa 2</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba 2 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automa 2</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba 2 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba automa 2</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba 2 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba 3 </t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba 3 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba 3 </t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba 3 Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Pruebaaa</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> PruebaaaAa Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Pruebaaa</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> PruebaaaAa Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Pruebaaa</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> PruebaaaAa Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Pruebaaa</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> PruebaaaAa Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Pruebaaa</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> PruebaaaAa Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Pruebaaa</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> PruebaaaAa Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Pruebaaa</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> PruebaaaAa Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Pruebaaa</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> PruebaaaAa Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Pruebaaa</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> PruebaaaAa Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Pruebaaa</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> PruebaaaAa Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Pruebaaa</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> PruebaaaAa Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Jolaaa</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Holaaa Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Jolaaa</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Holaaa Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Jolaaa</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Holaaa Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Jolaaa</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Holaaa Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Nico</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nico Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Nico</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nico Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Nico</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nico Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Nico</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nico Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Nico</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nico Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Nico</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nico Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Nico</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nico Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Nico</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nico Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Nico</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nico Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Nico</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nico Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Nico</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nico Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Nico</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nico Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Nico</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nico Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Nico</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nico Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Nico</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nico Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Nico</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nico Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Nico</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nico Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Nico</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nico Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Nico</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nico Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Nico</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nico Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Nico</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nico Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Nico</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nico Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Nico</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nico Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Nico</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nico Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Hol </t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Hol </t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Hol </t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Hol </t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Hol </t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Hol </t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Hol </t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Hol </t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Hol </t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Hol </t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Hol </t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Hol </t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Hol </t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Hol </t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Hol </t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Hol </t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Hol </t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Hol </t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Hol </t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Hol </t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Hol </t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Hol </t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Hol </t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Hol </t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Hol </t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Hol </t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Hol </t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Hol </t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Hol </t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Hol </t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Hol </t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Hol </t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Hol </t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Hol </t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Hol </t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📎 : Hol </t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📬 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📎 : Hol </t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📬 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📎 : Hol </t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📬 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📎 : Hol </t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📬 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📎 : Hol </t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📬 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📎 : Hol </t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📬 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📎 : Hol </t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📬 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📎 : Hol </t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📬 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📎 : Hol </t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📬 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📎 : Hol </t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📬 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📎 : Hol </t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📬 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📎 : Hol </t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📬 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📎 : Hol </t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📬 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📎 : Hol </t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📬 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📎 : Hol </t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📬 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📎 : Hol </t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📬 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📎 : Hol </t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📬 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📎 : Hol </t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📬 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📎 : Hol </t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📬 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📎 : Hol </t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📬 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📎 : Hol </t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📬 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📎 : Hol </t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📬 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📎 : Hol </t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📬 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📎 : Hol </t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📬 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📎 : Hol </t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📬 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📎 : Hol </t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📬 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📎 : Hol </t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📬 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📎 : Hol </t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📬 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📎 : Hol </t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📬 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📎 : Hol </t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📬 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hola Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📎 : Joan</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📬 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Joan Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📎 : Joan</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📬 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Joan Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Se hizo volvio al codigo anterior por problemas con la variable my_mail
</commit_message>
<xml_diff>
--- a/emails.xlsx
+++ b/emails.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D191"/>
+  <dimension ref="A1:D194"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4635,6 +4635,72 @@
         </is>
       </c>
     </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Joan</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Joan Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Joan</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Joan Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Joan</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Joan Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Se realizan pruebas para recoleccion del correo mas reciente en tiempo real
</commit_message>
<xml_diff>
--- a/emails.xlsx
+++ b/emails.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D194"/>
+  <dimension ref="A1:D232"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4701,6 +4701,842 @@
         </is>
       </c>
     </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Joan</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Joan Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Joan</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Joan Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Joan</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Joan Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Joan</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Joan Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Joan</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Joan Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Joan</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Joan Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Joan</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Joan Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Joan</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Joan Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Joan</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Joan Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Joan</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Joan Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Joan</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Joan Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Joan</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Joan Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Joan</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Joan Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Joan</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Joan Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Joan</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Joan Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Joan</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Joan Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Joan</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Joan Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Joan</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Joan Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Joan</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Joan Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Joan</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Joan Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Joan</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Joan Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Joan</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Joan Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Joan</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Joan Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Joan</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Joan Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Joan</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Joan Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Joan</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Joan Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Joan</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Joan Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Joan</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Joan Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Joan</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Joan Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : import datetime</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t xml:space="preserve">import datetime Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : import datetime</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t xml:space="preserve">import datetime Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : import datetime</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t xml:space="preserve">import datetime Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : import datetime</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t xml:space="preserve">import datetime Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : import datetime</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t xml:space="preserve">import datetime Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba </t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D229" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba </t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D230" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba </t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D231" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🔎 : Prueba </t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 📭 : Joan Martinez &lt;joan_martinez.olivares@hotmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prueba Obtener Outlook para iOS&lt;https://aka.ms/o0ukef&gt; </t>
+        </is>
+      </c>
+      <c r="D232" t="inlineStr">
+        <is>
+          <t>📩 NUEVO 📩</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>